<commit_message>
08/27/24 commit - added standings page and PDF of Weekly Standings from results spreadsheet
</commit_message>
<xml_diff>
--- a/public/results/Bottoms Up 2024 League Stats - Week 17.xlsx
+++ b/public/results/Bottoms Up 2024 League Stats - Week 17.xlsx
@@ -5,12 +5,12 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\mthut\iCloudDrive\Golf\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\DATA\CODE\golf-league-site\public\results\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{41A6B3F8-D882-4818-B302-028F99BFA4B0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{57274E2F-0A64-40B0-88E6-254835759E59}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="2340" yWindow="1335" windowWidth="23445" windowHeight="13665" firstSheet="2" activeTab="20" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="1590" yWindow="1815" windowWidth="23445" windowHeight="13665" firstSheet="1" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Template" sheetId="14" r:id="rId1"/>
@@ -57,7 +57,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="628" uniqueCount="132">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="631" uniqueCount="132">
   <si>
     <t>Karen</t>
   </si>
@@ -1932,6 +1932,51 @@
     <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="1" fontId="22" fillId="2" borderId="27" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" textRotation="90"/>
+    </xf>
+    <xf numFmtId="1" fontId="22" fillId="2" borderId="34" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" textRotation="90"/>
+    </xf>
+    <xf numFmtId="1" fontId="22" fillId="2" borderId="21" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" textRotation="90"/>
+    </xf>
+    <xf numFmtId="1" fontId="22" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" textRotation="90"/>
+    </xf>
+    <xf numFmtId="1" fontId="22" fillId="2" borderId="28" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" textRotation="90"/>
+    </xf>
+    <xf numFmtId="1" fontId="22" fillId="2" borderId="35" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" textRotation="90"/>
+    </xf>
+    <xf numFmtId="14" fontId="20" fillId="0" borderId="22" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="14" fontId="20" fillId="0" borderId="50" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="14" fontId="20" fillId="0" borderId="23" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="0" borderId="27" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="0" borderId="21" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="0" borderId="28" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="14" fontId="15" fillId="0" borderId="22" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -1943,6 +1988,42 @@
     </xf>
     <xf numFmtId="14" fontId="16" fillId="0" borderId="25" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="14" fontId="20" fillId="0" borderId="53" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="14" fontId="20" fillId="0" borderId="54" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="14" fontId="20" fillId="0" borderId="55" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="0" borderId="26" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="0" borderId="56" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="0" borderId="51" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="0" borderId="25" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="2" fontId="20" fillId="0" borderId="9" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="2" fontId="20" fillId="0" borderId="12" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="2" fontId="20" fillId="0" borderId="10" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="15" fillId="0" borderId="27" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -1982,87 +2063,6 @@
     </xf>
     <xf numFmtId="14" fontId="16" fillId="0" borderId="49" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="14" fontId="20" fillId="0" borderId="53" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="14" fontId="20" fillId="0" borderId="54" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="14" fontId="20" fillId="0" borderId="55" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="0" borderId="26" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="0" borderId="56" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="0" borderId="51" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="0" borderId="25" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="2" fontId="20" fillId="0" borderId="9" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="2" fontId="20" fillId="0" borderId="12" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="2" fontId="20" fillId="0" borderId="10" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="1" fontId="22" fillId="2" borderId="27" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" textRotation="90"/>
-    </xf>
-    <xf numFmtId="1" fontId="22" fillId="2" borderId="34" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" textRotation="90"/>
-    </xf>
-    <xf numFmtId="1" fontId="22" fillId="2" borderId="21" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" textRotation="90"/>
-    </xf>
-    <xf numFmtId="1" fontId="22" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" textRotation="90"/>
-    </xf>
-    <xf numFmtId="1" fontId="22" fillId="2" borderId="28" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" textRotation="90"/>
-    </xf>
-    <xf numFmtId="1" fontId="22" fillId="2" borderId="35" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" textRotation="90"/>
-    </xf>
-    <xf numFmtId="14" fontId="20" fillId="0" borderId="22" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="14" fontId="20" fillId="0" borderId="50" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="14" fontId="20" fillId="0" borderId="23" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="0" borderId="27" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="0" borderId="21" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="0" borderId="28" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="45" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -14807,8 +14807,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{6A1EE897-404D-4ADC-856A-1E864FE4E3AA}">
   <dimension ref="A1:AX25"/>
   <sheetViews>
-    <sheetView zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="AE4" sqref="AE4:AF20"/>
+    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="AJ24" sqref="AJ24"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -14839,7 +14839,8 @@
     <col min="24" max="24" width="6" hidden="1" customWidth="1"/>
     <col min="25" max="25" width="5.7109375" hidden="1" customWidth="1"/>
     <col min="26" max="26" width="6" hidden="1" customWidth="1"/>
-    <col min="27" max="38" width="7.42578125" customWidth="1"/>
+    <col min="27" max="34" width="7.42578125" hidden="1" customWidth="1"/>
+    <col min="35" max="38" width="7.42578125" customWidth="1"/>
     <col min="39" max="39" width="9.85546875" customWidth="1"/>
     <col min="40" max="40" width="9.140625" style="101"/>
     <col min="41" max="41" width="0" style="101" hidden="1" customWidth="1"/>
@@ -14854,212 +14855,212 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:50" s="1" customFormat="1" ht="14.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A1" s="173" t="s">
+      <c r="A1" s="200" t="s">
         <v>39</v>
       </c>
-      <c r="B1" s="174"/>
-      <c r="C1" s="179"/>
-      <c r="D1" s="182" t="s">
+      <c r="B1" s="201"/>
+      <c r="C1" s="206"/>
+      <c r="D1" s="209" t="s">
         <v>95</v>
       </c>
-      <c r="E1" s="169" t="s">
+      <c r="E1" s="184" t="s">
         <v>45</v>
       </c>
-      <c r="F1" s="170"/>
-      <c r="G1" s="169" t="s">
+      <c r="F1" s="185"/>
+      <c r="G1" s="184" t="s">
         <v>46</v>
       </c>
-      <c r="H1" s="170"/>
-      <c r="I1" s="169" t="s">
+      <c r="H1" s="185"/>
+      <c r="I1" s="184" t="s">
         <v>47</v>
       </c>
-      <c r="J1" s="170"/>
-      <c r="K1" s="169" t="s">
+      <c r="J1" s="185"/>
+      <c r="K1" s="184" t="s">
         <v>48</v>
       </c>
-      <c r="L1" s="170"/>
-      <c r="M1" s="169" t="s">
+      <c r="L1" s="185"/>
+      <c r="M1" s="184" t="s">
         <v>80</v>
       </c>
-      <c r="N1" s="170"/>
-      <c r="O1" s="169" t="s">
+      <c r="N1" s="185"/>
+      <c r="O1" s="184" t="s">
         <v>94</v>
       </c>
-      <c r="P1" s="170"/>
-      <c r="Q1" s="169" t="s">
+      <c r="P1" s="185"/>
+      <c r="Q1" s="184" t="s">
         <v>99</v>
       </c>
-      <c r="R1" s="170"/>
-      <c r="S1" s="169" t="s">
+      <c r="R1" s="185"/>
+      <c r="S1" s="184" t="s">
         <v>103</v>
       </c>
-      <c r="T1" s="170"/>
-      <c r="U1" s="169" t="s">
+      <c r="T1" s="185"/>
+      <c r="U1" s="184" t="s">
         <v>107</v>
       </c>
-      <c r="V1" s="170"/>
-      <c r="W1" s="169" t="s">
+      <c r="V1" s="185"/>
+      <c r="W1" s="184" t="s">
         <v>109</v>
       </c>
-      <c r="X1" s="170"/>
-      <c r="Y1" s="169" t="s">
+      <c r="X1" s="185"/>
+      <c r="Y1" s="184" t="s">
         <v>110</v>
       </c>
-      <c r="Z1" s="170"/>
-      <c r="AA1" s="169" t="s">
+      <c r="Z1" s="185"/>
+      <c r="AA1" s="184" t="s">
         <v>119</v>
       </c>
-      <c r="AB1" s="170"/>
-      <c r="AC1" s="169" t="s">
+      <c r="AB1" s="185"/>
+      <c r="AC1" s="184" t="s">
         <v>124</v>
       </c>
-      <c r="AD1" s="170"/>
-      <c r="AE1" s="169" t="s">
+      <c r="AD1" s="185"/>
+      <c r="AE1" s="184" t="s">
         <v>126</v>
       </c>
-      <c r="AF1" s="170"/>
-      <c r="AG1" s="169" t="s">
+      <c r="AF1" s="185"/>
+      <c r="AG1" s="184" t="s">
         <v>127</v>
       </c>
-      <c r="AH1" s="170"/>
-      <c r="AI1" s="169" t="s">
+      <c r="AH1" s="185"/>
+      <c r="AI1" s="184" t="s">
         <v>129</v>
       </c>
-      <c r="AJ1" s="170"/>
-      <c r="AK1" s="169" t="s">
+      <c r="AJ1" s="185"/>
+      <c r="AK1" s="184" t="s">
         <v>130</v>
       </c>
-      <c r="AL1" s="170"/>
-      <c r="AM1" s="210" t="s">
+      <c r="AL1" s="185"/>
+      <c r="AM1" s="181" t="s">
         <v>42</v>
       </c>
-      <c r="AN1" s="198" t="s">
+      <c r="AN1" s="197" t="s">
         <v>125</v>
       </c>
       <c r="AO1" s="127"/>
-      <c r="AP1" s="189" t="s">
+      <c r="AP1" s="188" t="s">
         <v>117</v>
       </c>
-      <c r="AQ1" s="190"/>
-      <c r="AR1" s="190"/>
-      <c r="AS1" s="191"/>
-      <c r="AT1" s="186" t="s">
+      <c r="AQ1" s="189"/>
+      <c r="AR1" s="189"/>
+      <c r="AS1" s="190"/>
+      <c r="AT1" s="178" t="s">
         <v>123</v>
       </c>
-      <c r="AU1" s="207" t="s">
+      <c r="AU1" s="175" t="s">
         <v>118</v>
       </c>
-      <c r="AV1" s="208"/>
-      <c r="AW1" s="208"/>
-      <c r="AX1" s="209"/>
+      <c r="AV1" s="176"/>
+      <c r="AW1" s="176"/>
+      <c r="AX1" s="177"/>
     </row>
     <row r="2" spans="1:50" s="1" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A2" s="175"/>
-      <c r="B2" s="176"/>
-      <c r="C2" s="180"/>
-      <c r="D2" s="183"/>
-      <c r="E2" s="171">
+      <c r="A2" s="202"/>
+      <c r="B2" s="203"/>
+      <c r="C2" s="207"/>
+      <c r="D2" s="210"/>
+      <c r="E2" s="186">
         <v>45418</v>
       </c>
-      <c r="F2" s="172"/>
-      <c r="G2" s="184">
+      <c r="F2" s="187"/>
+      <c r="G2" s="211">
         <v>45425</v>
       </c>
-      <c r="H2" s="185"/>
-      <c r="I2" s="184">
+      <c r="H2" s="212"/>
+      <c r="I2" s="211">
         <v>45432</v>
       </c>
-      <c r="J2" s="185"/>
-      <c r="K2" s="184">
+      <c r="J2" s="212"/>
+      <c r="K2" s="211">
         <v>45439</v>
       </c>
-      <c r="L2" s="185"/>
-      <c r="M2" s="184">
+      <c r="L2" s="212"/>
+      <c r="M2" s="211">
         <v>45446</v>
       </c>
-      <c r="N2" s="185"/>
-      <c r="O2" s="184">
+      <c r="N2" s="212"/>
+      <c r="O2" s="211">
         <v>45453</v>
       </c>
-      <c r="P2" s="185"/>
-      <c r="Q2" s="184">
+      <c r="P2" s="212"/>
+      <c r="Q2" s="211">
         <v>45460</v>
       </c>
-      <c r="R2" s="185"/>
-      <c r="S2" s="184">
+      <c r="R2" s="212"/>
+      <c r="S2" s="211">
         <v>45467</v>
       </c>
-      <c r="T2" s="185"/>
-      <c r="U2" s="184">
+      <c r="T2" s="212"/>
+      <c r="U2" s="211">
         <v>45474</v>
       </c>
-      <c r="V2" s="185"/>
-      <c r="W2" s="184">
+      <c r="V2" s="212"/>
+      <c r="W2" s="211">
         <v>45481</v>
       </c>
-      <c r="X2" s="185"/>
-      <c r="Y2" s="184">
+      <c r="X2" s="212"/>
+      <c r="Y2" s="211">
         <v>45488</v>
       </c>
-      <c r="Z2" s="185"/>
-      <c r="AA2" s="171">
+      <c r="Z2" s="212"/>
+      <c r="AA2" s="186">
         <v>45495</v>
       </c>
-      <c r="AB2" s="172"/>
-      <c r="AC2" s="171">
+      <c r="AB2" s="187"/>
+      <c r="AC2" s="186">
         <v>45502</v>
       </c>
-      <c r="AD2" s="172"/>
-      <c r="AE2" s="171">
+      <c r="AD2" s="187"/>
+      <c r="AE2" s="186">
         <v>45509</v>
       </c>
-      <c r="AF2" s="172"/>
-      <c r="AG2" s="171">
+      <c r="AF2" s="187"/>
+      <c r="AG2" s="186">
         <v>45516</v>
       </c>
-      <c r="AH2" s="172"/>
-      <c r="AI2" s="171">
+      <c r="AH2" s="187"/>
+      <c r="AI2" s="186">
         <v>45523</v>
       </c>
-      <c r="AJ2" s="172"/>
-      <c r="AK2" s="171">
+      <c r="AJ2" s="187"/>
+      <c r="AK2" s="186">
         <v>45530</v>
       </c>
-      <c r="AL2" s="172"/>
-      <c r="AM2" s="211"/>
-      <c r="AN2" s="199"/>
+      <c r="AL2" s="187"/>
+      <c r="AM2" s="182"/>
+      <c r="AN2" s="198"/>
       <c r="AO2" s="127"/>
-      <c r="AP2" s="192" t="s">
+      <c r="AP2" s="191" t="s">
         <v>98</v>
       </c>
-      <c r="AQ2" s="194" t="s">
+      <c r="AQ2" s="193" t="s">
         <v>116</v>
       </c>
-      <c r="AR2" s="194" t="s">
+      <c r="AR2" s="193" t="s">
         <v>43</v>
       </c>
-      <c r="AS2" s="196" t="s">
+      <c r="AS2" s="195" t="s">
         <v>70</v>
       </c>
-      <c r="AT2" s="187"/>
-      <c r="AU2" s="186" t="s">
+      <c r="AT2" s="179"/>
+      <c r="AU2" s="178" t="s">
         <v>98</v>
       </c>
-      <c r="AV2" s="186" t="s">
+      <c r="AV2" s="178" t="s">
         <v>116</v>
       </c>
-      <c r="AW2" s="186" t="s">
+      <c r="AW2" s="178" t="s">
         <v>43</v>
       </c>
-      <c r="AX2" s="186" t="s">
+      <c r="AX2" s="178" t="s">
         <v>70</v>
       </c>
     </row>
     <row r="3" spans="1:50" s="1" customFormat="1" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A3" s="177"/>
-      <c r="B3" s="178"/>
-      <c r="C3" s="181"/>
-      <c r="D3" s="183"/>
+      <c r="A3" s="204"/>
+      <c r="B3" s="205"/>
+      <c r="C3" s="208"/>
+      <c r="D3" s="210"/>
       <c r="E3" s="60" t="s">
         <v>28</v>
       </c>
@@ -15162,18 +15163,18 @@
       <c r="AL3" s="61" t="s">
         <v>29</v>
       </c>
-      <c r="AM3" s="212"/>
-      <c r="AN3" s="200"/>
+      <c r="AM3" s="183"/>
+      <c r="AN3" s="199"/>
       <c r="AO3" s="127"/>
-      <c r="AP3" s="193"/>
-      <c r="AQ3" s="195"/>
-      <c r="AR3" s="195"/>
-      <c r="AS3" s="197"/>
-      <c r="AT3" s="188"/>
-      <c r="AU3" s="187"/>
-      <c r="AV3" s="188"/>
-      <c r="AW3" s="187"/>
-      <c r="AX3" s="188"/>
+      <c r="AP3" s="192"/>
+      <c r="AQ3" s="194"/>
+      <c r="AR3" s="194"/>
+      <c r="AS3" s="196"/>
+      <c r="AT3" s="180"/>
+      <c r="AU3" s="179"/>
+      <c r="AV3" s="180"/>
+      <c r="AW3" s="179"/>
+      <c r="AX3" s="180"/>
     </row>
     <row r="4" spans="1:50" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A4" s="64" t="s">
@@ -15243,16 +15244,16 @@
       </c>
       <c r="AC4" s="146"/>
       <c r="AD4" s="70"/>
-      <c r="AE4" s="201" t="s">
+      <c r="AE4" s="169" t="s">
         <v>128</v>
       </c>
-      <c r="AF4" s="202"/>
+      <c r="AF4" s="170"/>
       <c r="AG4" s="146"/>
       <c r="AH4" s="70"/>
-      <c r="AI4" s="201" t="s">
+      <c r="AI4" s="169" t="s">
         <v>128</v>
       </c>
-      <c r="AJ4" s="202"/>
+      <c r="AJ4" s="170"/>
       <c r="AK4" s="121">
         <v>57</v>
       </c>
@@ -15384,12 +15385,12 @@
       <c r="AD5" s="79">
         <v>21</v>
       </c>
-      <c r="AE5" s="203"/>
-      <c r="AF5" s="204"/>
+      <c r="AE5" s="171"/>
+      <c r="AF5" s="172"/>
       <c r="AG5" s="80"/>
       <c r="AH5" s="81"/>
-      <c r="AI5" s="203"/>
-      <c r="AJ5" s="204"/>
+      <c r="AI5" s="171"/>
+      <c r="AJ5" s="172"/>
       <c r="AK5" s="78">
         <v>53</v>
       </c>
@@ -15525,16 +15526,16 @@
       <c r="AD6" s="142">
         <v>18</v>
       </c>
-      <c r="AE6" s="203"/>
-      <c r="AF6" s="204"/>
+      <c r="AE6" s="171"/>
+      <c r="AF6" s="172"/>
       <c r="AG6" s="86">
         <v>49</v>
       </c>
       <c r="AH6" s="79">
         <v>18</v>
       </c>
-      <c r="AI6" s="203"/>
-      <c r="AJ6" s="204"/>
+      <c r="AI6" s="171"/>
+      <c r="AJ6" s="172"/>
       <c r="AK6" s="141">
         <v>47</v>
       </c>
@@ -15660,16 +15661,16 @@
       <c r="AD7" s="79">
         <v>19</v>
       </c>
-      <c r="AE7" s="203"/>
-      <c r="AF7" s="204"/>
+      <c r="AE7" s="171"/>
+      <c r="AF7" s="172"/>
       <c r="AG7" s="88">
         <v>39</v>
       </c>
       <c r="AH7" s="79">
         <v>17</v>
       </c>
-      <c r="AI7" s="203"/>
-      <c r="AJ7" s="204"/>
+      <c r="AI7" s="171"/>
+      <c r="AJ7" s="172"/>
       <c r="AK7" s="86">
         <v>37</v>
       </c>
@@ -15801,16 +15802,16 @@
       <c r="AD8" s="79">
         <v>21</v>
       </c>
-      <c r="AE8" s="203"/>
-      <c r="AF8" s="204"/>
+      <c r="AE8" s="171"/>
+      <c r="AF8" s="172"/>
       <c r="AG8" s="78">
         <v>58</v>
       </c>
       <c r="AH8" s="79">
         <v>17</v>
       </c>
-      <c r="AI8" s="203"/>
-      <c r="AJ8" s="204"/>
+      <c r="AI8" s="171"/>
+      <c r="AJ8" s="172"/>
       <c r="AK8" s="78">
         <v>51</v>
       </c>
@@ -15906,16 +15907,16 @@
       <c r="AD9" s="79">
         <v>17</v>
       </c>
-      <c r="AE9" s="203"/>
-      <c r="AF9" s="204"/>
+      <c r="AE9" s="171"/>
+      <c r="AF9" s="172"/>
       <c r="AG9" s="78">
         <v>57</v>
       </c>
       <c r="AH9" s="79">
         <v>20</v>
       </c>
-      <c r="AI9" s="203"/>
-      <c r="AJ9" s="204"/>
+      <c r="AI9" s="171"/>
+      <c r="AJ9" s="172"/>
       <c r="AK9" s="80"/>
       <c r="AL9" s="81"/>
       <c r="AM9" s="72">
@@ -16032,16 +16033,16 @@
       <c r="AD10" s="79">
         <v>14</v>
       </c>
-      <c r="AE10" s="203"/>
-      <c r="AF10" s="204"/>
+      <c r="AE10" s="171"/>
+      <c r="AF10" s="172"/>
       <c r="AG10" s="78">
         <v>41</v>
       </c>
       <c r="AH10" s="79">
         <v>22</v>
       </c>
-      <c r="AI10" s="203"/>
-      <c r="AJ10" s="204"/>
+      <c r="AI10" s="171"/>
+      <c r="AJ10" s="172"/>
       <c r="AK10" s="78">
         <v>49</v>
       </c>
@@ -16161,16 +16162,16 @@
       <c r="AD11" s="79">
         <v>16</v>
       </c>
-      <c r="AE11" s="203"/>
-      <c r="AF11" s="204"/>
+      <c r="AE11" s="171"/>
+      <c r="AF11" s="172"/>
       <c r="AG11" s="78">
         <v>49</v>
       </c>
       <c r="AH11" s="79">
         <v>16</v>
       </c>
-      <c r="AI11" s="203"/>
-      <c r="AJ11" s="204"/>
+      <c r="AI11" s="171"/>
+      <c r="AJ11" s="172"/>
       <c r="AK11" s="88">
         <v>44</v>
       </c>
@@ -16308,16 +16309,16 @@
       <c r="AD12" s="79">
         <v>21</v>
       </c>
-      <c r="AE12" s="203"/>
-      <c r="AF12" s="204"/>
+      <c r="AE12" s="171"/>
+      <c r="AF12" s="172"/>
       <c r="AG12" s="78">
         <v>59</v>
       </c>
       <c r="AH12" s="79">
         <v>12</v>
       </c>
-      <c r="AI12" s="203"/>
-      <c r="AJ12" s="204"/>
+      <c r="AI12" s="171"/>
+      <c r="AJ12" s="172"/>
       <c r="AK12" s="78">
         <v>57</v>
       </c>
@@ -16447,16 +16448,16 @@
       <c r="AD13" s="79">
         <v>15</v>
       </c>
-      <c r="AE13" s="203"/>
-      <c r="AF13" s="204"/>
+      <c r="AE13" s="171"/>
+      <c r="AF13" s="172"/>
       <c r="AG13" s="78">
         <v>52</v>
       </c>
       <c r="AH13" s="79">
         <v>18</v>
       </c>
-      <c r="AI13" s="203"/>
-      <c r="AJ13" s="204"/>
+      <c r="AI13" s="171"/>
+      <c r="AJ13" s="172"/>
       <c r="AK13" s="78">
         <v>56</v>
       </c>
@@ -16576,16 +16577,16 @@
       <c r="AD14" s="79">
         <v>13</v>
       </c>
-      <c r="AE14" s="203"/>
-      <c r="AF14" s="204"/>
+      <c r="AE14" s="171"/>
+      <c r="AF14" s="172"/>
       <c r="AG14" s="78">
         <v>48</v>
       </c>
       <c r="AH14" s="79">
         <v>19</v>
       </c>
-      <c r="AI14" s="203"/>
-      <c r="AJ14" s="204"/>
+      <c r="AI14" s="171"/>
+      <c r="AJ14" s="172"/>
       <c r="AK14" s="78">
         <v>50</v>
       </c>
@@ -16693,16 +16694,16 @@
       <c r="AB15" s="81"/>
       <c r="AC15" s="80"/>
       <c r="AD15" s="81"/>
-      <c r="AE15" s="203"/>
-      <c r="AF15" s="204"/>
+      <c r="AE15" s="171"/>
+      <c r="AF15" s="172"/>
       <c r="AG15" s="78">
         <v>54</v>
       </c>
       <c r="AH15" s="79">
         <v>15</v>
       </c>
-      <c r="AI15" s="203"/>
-      <c r="AJ15" s="204"/>
+      <c r="AI15" s="171"/>
+      <c r="AJ15" s="172"/>
       <c r="AK15" s="80"/>
       <c r="AL15" s="81"/>
       <c r="AM15" s="72">
@@ -16828,12 +16829,12 @@
       <c r="AB16" s="81"/>
       <c r="AC16" s="80"/>
       <c r="AD16" s="81"/>
-      <c r="AE16" s="203"/>
-      <c r="AF16" s="204"/>
+      <c r="AE16" s="171"/>
+      <c r="AF16" s="172"/>
       <c r="AG16" s="80"/>
       <c r="AH16" s="81"/>
-      <c r="AI16" s="203"/>
-      <c r="AJ16" s="204"/>
+      <c r="AI16" s="171"/>
+      <c r="AJ16" s="172"/>
       <c r="AK16" s="80"/>
       <c r="AL16" s="81"/>
       <c r="AM16" s="72">
@@ -16919,12 +16920,12 @@
       <c r="AB17" s="81"/>
       <c r="AC17" s="80"/>
       <c r="AD17" s="81"/>
-      <c r="AE17" s="203"/>
-      <c r="AF17" s="204"/>
+      <c r="AE17" s="171"/>
+      <c r="AF17" s="172"/>
       <c r="AG17" s="80"/>
       <c r="AH17" s="81"/>
-      <c r="AI17" s="203"/>
-      <c r="AJ17" s="204"/>
+      <c r="AI17" s="171"/>
+      <c r="AJ17" s="172"/>
       <c r="AK17" s="80"/>
       <c r="AL17" s="81"/>
       <c r="AM17" s="72">
@@ -17010,12 +17011,12 @@
       <c r="AB18" s="81"/>
       <c r="AC18" s="80"/>
       <c r="AD18" s="81"/>
-      <c r="AE18" s="203"/>
-      <c r="AF18" s="204"/>
+      <c r="AE18" s="171"/>
+      <c r="AF18" s="172"/>
       <c r="AG18" s="80"/>
       <c r="AH18" s="81"/>
-      <c r="AI18" s="203"/>
-      <c r="AJ18" s="204"/>
+      <c r="AI18" s="171"/>
+      <c r="AJ18" s="172"/>
       <c r="AK18" s="80"/>
       <c r="AL18" s="81"/>
       <c r="AM18" s="72">
@@ -17114,12 +17115,12 @@
       <c r="AB19" s="81"/>
       <c r="AC19" s="80"/>
       <c r="AD19" s="81"/>
-      <c r="AE19" s="203"/>
-      <c r="AF19" s="204"/>
+      <c r="AE19" s="171"/>
+      <c r="AF19" s="172"/>
       <c r="AG19" s="80"/>
       <c r="AH19" s="81"/>
-      <c r="AI19" s="203"/>
-      <c r="AJ19" s="204"/>
+      <c r="AI19" s="171"/>
+      <c r="AJ19" s="172"/>
       <c r="AK19" s="80"/>
       <c r="AL19" s="81"/>
       <c r="AM19" s="72">
@@ -17209,12 +17210,12 @@
       </c>
       <c r="AC20" s="80"/>
       <c r="AD20" s="81"/>
-      <c r="AE20" s="205"/>
-      <c r="AF20" s="206"/>
+      <c r="AE20" s="173"/>
+      <c r="AF20" s="174"/>
       <c r="AG20" s="80"/>
       <c r="AH20" s="81"/>
-      <c r="AI20" s="205"/>
-      <c r="AJ20" s="206"/>
+      <c r="AI20" s="173"/>
+      <c r="AJ20" s="174"/>
       <c r="AK20" s="80"/>
       <c r="AL20" s="81"/>
       <c r="AM20" s="72">
@@ -17376,7 +17377,9 @@
       <c r="AC23" s="139"/>
       <c r="AE23" s="139"/>
       <c r="AG23" s="139"/>
-      <c r="AI23" s="139"/>
+      <c r="AI23" s="139" t="s">
+        <v>32</v>
+      </c>
       <c r="AK23" s="139"/>
     </row>
     <row r="24" spans="1:50" x14ac:dyDescent="0.25">
@@ -17392,7 +17395,9 @@
       <c r="AC24" s="138"/>
       <c r="AE24" s="138"/>
       <c r="AG24" s="138"/>
-      <c r="AI24" s="138"/>
+      <c r="AI24" s="138" t="s">
+        <v>33</v>
+      </c>
       <c r="AK24" s="138"/>
     </row>
     <row r="25" spans="1:50" x14ac:dyDescent="0.25">
@@ -17409,7 +17414,9 @@
       <c r="AE25" s="140"/>
       <c r="AG25" s="140"/>
       <c r="AH25" s="152"/>
-      <c r="AI25" s="140"/>
+      <c r="AI25" s="140" t="s">
+        <v>105</v>
+      </c>
       <c r="AK25" s="140"/>
       <c r="AL25" s="152"/>
     </row>
@@ -17419,28 +17426,20 @@
     <sortCondition ref="AN4:AN20"/>
   </sortState>
   <mergeCells count="52">
-    <mergeCell ref="AE4:AF20"/>
-    <mergeCell ref="AU1:AX1"/>
-    <mergeCell ref="AU2:AU3"/>
-    <mergeCell ref="AV2:AV3"/>
-    <mergeCell ref="AW2:AW3"/>
-    <mergeCell ref="AX2:AX3"/>
-    <mergeCell ref="AM1:AM3"/>
-    <mergeCell ref="AI4:AJ20"/>
-    <mergeCell ref="AK1:AL1"/>
-    <mergeCell ref="AK2:AL2"/>
-    <mergeCell ref="AT1:AT3"/>
-    <mergeCell ref="AA1:AB1"/>
-    <mergeCell ref="AA2:AB2"/>
-    <mergeCell ref="AP1:AS1"/>
-    <mergeCell ref="AP2:AP3"/>
-    <mergeCell ref="AQ2:AQ3"/>
-    <mergeCell ref="AR2:AR3"/>
-    <mergeCell ref="AS2:AS3"/>
-    <mergeCell ref="AN1:AN3"/>
-    <mergeCell ref="AE1:AF1"/>
-    <mergeCell ref="AE2:AF2"/>
-    <mergeCell ref="AG1:AH1"/>
+    <mergeCell ref="M1:N1"/>
+    <mergeCell ref="O1:P1"/>
+    <mergeCell ref="E2:F2"/>
+    <mergeCell ref="AI1:AJ1"/>
+    <mergeCell ref="AI2:AJ2"/>
+    <mergeCell ref="AC1:AD1"/>
+    <mergeCell ref="AC2:AD2"/>
+    <mergeCell ref="AG2:AH2"/>
+    <mergeCell ref="Y2:Z2"/>
+    <mergeCell ref="Y1:Z1"/>
+    <mergeCell ref="W2:X2"/>
+    <mergeCell ref="W1:X1"/>
+    <mergeCell ref="K2:L2"/>
+    <mergeCell ref="M2:N2"/>
     <mergeCell ref="A1:B3"/>
     <mergeCell ref="C1:C3"/>
     <mergeCell ref="D1:D3"/>
@@ -17457,23 +17456,32 @@
     <mergeCell ref="U1:V1"/>
     <mergeCell ref="G2:H2"/>
     <mergeCell ref="I2:J2"/>
-    <mergeCell ref="M1:N1"/>
-    <mergeCell ref="O1:P1"/>
-    <mergeCell ref="E2:F2"/>
-    <mergeCell ref="AI1:AJ1"/>
-    <mergeCell ref="AI2:AJ2"/>
-    <mergeCell ref="AC1:AD1"/>
-    <mergeCell ref="AC2:AD2"/>
-    <mergeCell ref="AG2:AH2"/>
-    <mergeCell ref="Y2:Z2"/>
-    <mergeCell ref="Y1:Z1"/>
-    <mergeCell ref="W2:X2"/>
-    <mergeCell ref="W1:X1"/>
-    <mergeCell ref="K2:L2"/>
-    <mergeCell ref="M2:N2"/>
+    <mergeCell ref="AA1:AB1"/>
+    <mergeCell ref="AA2:AB2"/>
+    <mergeCell ref="AP1:AS1"/>
+    <mergeCell ref="AP2:AP3"/>
+    <mergeCell ref="AQ2:AQ3"/>
+    <mergeCell ref="AR2:AR3"/>
+    <mergeCell ref="AS2:AS3"/>
+    <mergeCell ref="AN1:AN3"/>
+    <mergeCell ref="AE1:AF1"/>
+    <mergeCell ref="AE2:AF2"/>
+    <mergeCell ref="AG1:AH1"/>
+    <mergeCell ref="AE4:AF20"/>
+    <mergeCell ref="AU1:AX1"/>
+    <mergeCell ref="AU2:AU3"/>
+    <mergeCell ref="AV2:AV3"/>
+    <mergeCell ref="AW2:AW3"/>
+    <mergeCell ref="AX2:AX3"/>
+    <mergeCell ref="AM1:AM3"/>
+    <mergeCell ref="AI4:AJ20"/>
+    <mergeCell ref="AK1:AL1"/>
+    <mergeCell ref="AK2:AL2"/>
+    <mergeCell ref="AT1:AT3"/>
   </mergeCells>
   <phoneticPr fontId="19" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="landscape" horizontalDpi="0" verticalDpi="0" r:id="rId1"/>
   <webPublishItems count="1">
     <webPublishItem id="24146" divId="Bottoms Up 2024 League Stats - Week 11_24146" sourceType="sheet" destinationFile="C:\DATA\CODE\golf-league-site\public\results\Bottoms Up 2024 League Stats - Week 11.htm" title="WEEK 11" autoRepublish="1"/>
   </webPublishItems>
@@ -17525,7 +17533,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D7815779-C5C7-4C22-8371-169A5BC8E021}">
   <dimension ref="A1:Z26"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
+    <sheetView zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
       <selection activeCell="T33" sqref="T33"/>
     </sheetView>
   </sheetViews>

</xml_diff>